<commit_message>
fix date formats in sample files
</commit_message>
<xml_diff>
--- a/AirportSystem/SampleInputFiles/sample.xlsx
+++ b/AirportSystem/SampleInputFiles/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>sheduledTime</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>A5</t>
+  </si>
+  <si>
+    <t>2017-06-07T13:34:08.0039447-05:00</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
@@ -528,8 +531,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>42891.670219907406</v>
+      <c r="A2" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Added Working Excel Deserializer
</commit_message>
<xml_diff>
--- a/AirportSystem/SampleInputFiles/sample.xlsx
+++ b/AirportSystem/SampleInputFiles/sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>sheduledTime</t>
   </si>
@@ -82,6 +82,42 @@
   </si>
   <si>
     <t>2017-06-07T13:34:08.0039447-05:00</t>
+  </si>
+  <si>
+    <t>2017-06-07T13:34:08.0039447-05:01</t>
+  </si>
+  <si>
+    <t>E176</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>2017-06-07T13:34:08.0039447-05:02</t>
+  </si>
+  <si>
+    <t>E177</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>2017-06-07T13:34:08.0039447-05:03</t>
+  </si>
+  <si>
+    <t>E178</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>2017-06-07T13:34:08.0039447-05:04</t>
+  </si>
+  <si>
+    <t>E179</t>
+  </si>
+  <si>
+    <t>A9</t>
   </si>
 </sst>
 </file>
@@ -156,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,10 +200,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -179,6 +218,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -227,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,42 +572,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>80</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>2005</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5">
+        <v>81</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5">
+        <v>82</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2007</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="5">
+        <v>83</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2008</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="5">
+        <v>84</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2009</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>